<commit_message>
Quick Employee onboard revised excel , adding new column  active in users table
</commit_message>
<xml_diff>
--- a/public/assets/sample_employeeBulkQuickOnboarding.xlsx
+++ b/public/assets/sample_employeeBulkQuickOnboarding.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Employee Name</t>
   </si>
@@ -19,29 +19,70 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Task1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>rahul.sgsits2015</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
-        <u/>
-      </rPr>
-      <t>@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Task2</t>
+    <t>DOJ</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>HRA</t>
+  </si>
+  <si>
+    <t>Statutory Bonus</t>
+  </si>
+  <si>
+    <t>Child Education Allowance</t>
+  </si>
+  <si>
+    <t>Food Coupon</t>
+  </si>
+  <si>
+    <t>LTA</t>
+  </si>
+  <si>
+    <t>Special Allowance</t>
+  </si>
+  <si>
+    <t>Other Allowance</t>
+  </si>
+  <si>
+    <t>EPF Employer Contribution</t>
+  </si>
+  <si>
+    <t>ESIC Employer Contribution</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Graduity</t>
+  </si>
+  <si>
+    <t>EPf Employee</t>
+  </si>
+  <si>
+    <t>ESIC Employee</t>
+  </si>
+  <si>
+    <t>Professional Tax</t>
+  </si>
+  <si>
+    <t>Labour Welfare Fund</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>rahul.sgsits2015@gmail.com</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
   <si>
     <t>voidmaxtech@gmail.com</t>
@@ -51,7 +92,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -63,38 +107,50 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -313,7 +369,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.63"/>
+    <col customWidth="1" min="1" max="3" width="12.63"/>
+    <col customWidth="1" min="4" max="4" width="12.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -323,30 +380,198 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2">
+        <v>35890.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8.776648329E9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>12000.0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>100.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="2">
+        <v>35890.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8.776648329E9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1">
+        <v>12000.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>100.0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Employee Code in Quick Bulk Uploading.
</commit_message>
<xml_diff>
--- a/public/assets/sample_employeeBulkQuickOnboarding.xlsx
+++ b/public/assets/sample_employeeBulkQuickOnboarding.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">Employee Code</t>
+  </si>
   <si>
     <t xml:space="preserve">Employee Name</t>
   </si>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">Labour Welfare Fund</t>
   </si>
   <si>
+    <t xml:space="preserve">ABS1001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emp 1</t>
   </si>
   <si>
@@ -92,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emp 2</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -129,6 +132,14 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -144,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -152,6 +163,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -178,11 +196,31 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,10 +231,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -216,22 +250,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.88"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -240,192 +274,155 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="n">
         <v>32968</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="E2" s="8" t="n">
         <v>1111111111</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="n">
         <v>12000</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="6" t="n">
         <v>2000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="I2" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="J2" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="L2" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="M2" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="N2" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="N2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="S2" s="1" t="n">
+      <c r="O2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="P2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="R2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="S2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="T2" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="T2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="U2" s="1" t="n">
+      <c r="U2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="V2" s="6" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>32968</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>2222222222</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>12000</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="U3" s="1" t="n">
-        <v>100</v>
-      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="test@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="test@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="test@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
excel sheet updated bulk and quick
</commit_message>
<xml_diff>
--- a/public/assets/sample_employeeBulkQuickOnboarding.xlsx
+++ b/public/assets/sample_employeeBulkQuickOnboarding.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="0"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -54,9 +48,6 @@
     <t xml:space="preserve">Designation </t>
   </si>
   <si>
-    <t xml:space="preserve">Reporting Manager Code </t>
-  </si>
-  <si>
     <t>Basic</t>
   </si>
   <si>
@@ -111,35 +102,32 @@
     <t>Srinivasan</t>
   </si>
   <si>
-    <t>XXXX@gmail.com</t>
-  </si>
-  <si>
-    <t>YY/MM/DD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Text value </t>
   </si>
   <si>
     <t>Nil</t>
+  </si>
+  <si>
+    <t>dd-mm-yyyy</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>L1 Manager Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -150,7 +138,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -167,7 +155,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39998000860214233"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,121 +181,28 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -362,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -414,7 +309,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -608,45 +503,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AD64F6-6E6E-43B6-912D-9C63CA2109D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.142857142857142" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.285714285714285" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.571428571428573" customWidth="1"/>
-    <col min="4" max="4" width="14.428571428571429" customWidth="1"/>
-    <col min="5" max="5" width="19.285714285714285" customWidth="1"/>
-    <col min="6" max="6" width="18.571428571428573" customWidth="1"/>
-    <col min="7" max="7" width="25.142857142857142" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.714285714285715" customWidth="1"/>
-    <col min="11" max="11" width="26.285714285714285" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.285714285714286" customWidth="1"/>
-    <col min="14" max="14" width="17.428571428571427" customWidth="1"/>
-    <col min="15" max="15" width="15.571428571428571" customWidth="1"/>
-    <col min="16" max="16" width="28.714285714285715" customWidth="1"/>
-    <col min="17" max="17" width="30.857142857142858" customWidth="1"/>
-    <col min="18" max="18" width="14.285714285714286" customWidth="1"/>
-    <col min="19" max="19" width="13.428571428571429" customWidth="1"/>
-    <col min="20" max="20" width="15.428571428571429" customWidth="1"/>
-    <col min="21" max="21" width="18.285714285714285" customWidth="1"/>
-    <col min="22" max="22" width="16.285714285714285" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.714285714285715" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="28.7109375" customWidth="1"/>
+    <col min="17" max="17" width="30.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="15.6">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -666,78 +561,78 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="14.4">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>26</v>
       </c>
       <c r="E2">
-        <v>9876543245</v>
+        <v>1234567890</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -770,10 +665,10 @@
         <v>1000</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T2">
         <v>1000</v>
@@ -790,9 +685,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="XXXX@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="1" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>